<commit_message>
.gitignore is now working 1
</commit_message>
<xml_diff>
--- a/Scrum Meeting Log.xlsx
+++ b/Scrum Meeting Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byu77\Documents\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E071BAC8-9DBB-489F-A95A-10BE02B8A920}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6153218E-653C-44B5-9AA4-C4AEA4BED229}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9398" xr2:uid="{4F85B5DE-145D-407F-AE0B-3658DEF44FEC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Day</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Ben Change 2</t>
+  </si>
+  <si>
+    <t>Ben Change 3</t>
   </si>
 </sst>
 </file>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64DA117A-A919-47F8-9C06-21B6E1A75659}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -460,7 +463,7 @@
     <col min="2" max="2" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -473,13 +476,16 @@
       <c r="G1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="B2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -487,32 +493,32 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="B5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="B6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="B7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="B8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="B9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -520,7 +526,7 @@
         <v>43442</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -528,7 +534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -536,7 +542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>4</v>
       </c>

</xml_diff>